<commit_message>
AttachSubDirectories upgrade to folderNode, GetDescription() method to aceAuthorNotation data objectetc.
</commit_message>
<xml_diff>
--- a/TEST/TableTest/dt_exporttext.xlsx_custom_table_entry.xlsx
+++ b/TEST/TableTest/dt_exporttext.xlsx_custom_table_entry.xlsx
@@ -57,34 +57,34 @@
     <t>%</t>
   </si>
   <si>
-    <t>h6f9008g6iyl249</t>
-  </si>
-  <si>
-    <t>jvya05a7k917i08</t>
-  </si>
-  <si>
-    <t>kx46jvh531m9d60</t>
-  </si>
-  <si>
-    <t>eu3kmi38nt54825</t>
+    <t>mesu5p700d3ja57</t>
+  </si>
+  <si>
+    <t>67rgxmn16wdl1t3</t>
+  </si>
+  <si>
+    <t>978vx4h4n1d0t12</t>
+  </si>
+  <si>
+    <t>qtp57advs3xssvx</t>
   </si>
   <si>
     <t>T2</t>
   </si>
   <si>
-    <t>9lvg2gbx44a7n8x</t>
-  </si>
-  <si>
-    <t>160n1w84nsgd8iu</t>
-  </si>
-  <si>
-    <t>qr9kb9xesxd536r</t>
+    <t>x00hb59d369oi73</t>
+  </si>
+  <si>
+    <t>ty2if8tqb09qg33</t>
+  </si>
+  <si>
+    <t>j91su458oloof53</t>
   </si>
   <si>
     <t>T1</t>
   </si>
   <si>
-    <t>9e73t0ij3j7f0nf</t>
+    <t>7e4m3n9on40nvc6</t>
   </si>
   <si>
     <t>T3</t>

</xml_diff>

<commit_message>
error fixes and graph report update
</commit_message>
<xml_diff>
--- a/TEST/TableTest/dt_exporttext.xlsx_custom_table_entry.xlsx
+++ b/TEST/TableTest/dt_exporttext.xlsx_custom_table_entry.xlsx
@@ -57,34 +57,34 @@
     <t>%</t>
   </si>
   <si>
-    <t>bfkgt1v508g78dc</t>
-  </si>
-  <si>
-    <t>nm3je437823p8rd</t>
-  </si>
-  <si>
-    <t>9228iq6ak1qett7</t>
-  </si>
-  <si>
-    <t>oes769417v92h69</t>
+    <t>r287445k397636v</t>
+  </si>
+  <si>
+    <t>o0k701899833syn</t>
+  </si>
+  <si>
+    <t>29k5z09pu083z17</t>
+  </si>
+  <si>
+    <t>ral65f969l2i021</t>
   </si>
   <si>
     <t>T2</t>
   </si>
   <si>
-    <t>cnt5no0f0fjuc8y</t>
-  </si>
-  <si>
-    <t>a681e9wau7ms74f</t>
-  </si>
-  <si>
-    <t>skj148025c83707</t>
+    <t>721775c46nu5dbb</t>
+  </si>
+  <si>
+    <t>4526v8k0ema390l</t>
+  </si>
+  <si>
+    <t>6744r3n65e16u49</t>
   </si>
   <si>
     <t>T1</t>
   </si>
   <si>
-    <t>g9v00zol2n2hf05</t>
+    <t>59iiat6631exp92</t>
   </si>
   <si>
     <t>T3</t>

</xml_diff>

<commit_message>
heat mapping of image files, bug fixing
</commit_message>
<xml_diff>
--- a/TEST/TableTest/dt_exporttext.xlsx_custom_table_entry.xlsx
+++ b/TEST/TableTest/dt_exporttext.xlsx_custom_table_entry.xlsx
@@ -57,34 +57,34 @@
     <t>%</t>
   </si>
   <si>
-    <t>85v2za4dbhq58p4</t>
-  </si>
-  <si>
-    <t>qm0jg6cax1xh3j2</t>
-  </si>
-  <si>
-    <t>38512183psg5j82</t>
-  </si>
-  <si>
-    <t>924qsgqdg3oc303</t>
+    <t>ui9v547jxpt9of6</t>
+  </si>
+  <si>
+    <t>6xmay00ev2l4pl1</t>
+  </si>
+  <si>
+    <t>1f1s9j33q3lll85</t>
+  </si>
+  <si>
+    <t>rdo4e4x959n4262</t>
   </si>
   <si>
     <t>T2</t>
   </si>
   <si>
-    <t>1ny3foo2da3lk4f</t>
-  </si>
-  <si>
-    <t>1995i0mpnpk5q8w</t>
-  </si>
-  <si>
-    <t>d0d26q9zqni84k1</t>
+    <t>ka5njrmwml2tw7y</t>
+  </si>
+  <si>
+    <t>225el2d7iyhk1i6</t>
+  </si>
+  <si>
+    <t>4f1z9ba31h53526</t>
   </si>
   <si>
     <t>T1</t>
   </si>
   <si>
-    <t>0mlzzb8p7ki87bx</t>
+    <t>ds2d4310f2yqd8a</t>
   </si>
   <si>
     <t>T3</t>

</xml_diff>

<commit_message>
SVG api, MXGraph and Dia support
</commit_message>
<xml_diff>
--- a/TEST/TableTest/dt_exporttext.xlsx_custom_table_entry.xlsx
+++ b/TEST/TableTest/dt_exporttext.xlsx_custom_table_entry.xlsx
@@ -57,34 +57,34 @@
     <t>%</t>
   </si>
   <si>
-    <t>ui9v547jxpt9of6</t>
-  </si>
-  <si>
-    <t>6xmay00ev2l4pl1</t>
-  </si>
-  <si>
-    <t>1f1s9j33q3lll85</t>
-  </si>
-  <si>
-    <t>rdo4e4x959n4262</t>
+    <t>4b44pz84e13934k</t>
+  </si>
+  <si>
+    <t>15ikn58z719910o</t>
+  </si>
+  <si>
+    <t>1b1ejz1ds8x9782</t>
+  </si>
+  <si>
+    <t>ir6w36l8441kx3f</t>
   </si>
   <si>
     <t>T2</t>
   </si>
   <si>
-    <t>ka5njrmwml2tw7y</t>
-  </si>
-  <si>
-    <t>225el2d7iyhk1i6</t>
-  </si>
-  <si>
-    <t>4f1z9ba31h53526</t>
+    <t>4a73q62w180m377</t>
+  </si>
+  <si>
+    <t>ut3j26acgfkqnuo</t>
+  </si>
+  <si>
+    <t>061atd70d46krvg</t>
   </si>
   <si>
     <t>T1</t>
   </si>
   <si>
-    <t>ds2d4310f2yqd8a</t>
+    <t>p9x3i35263e933x</t>
   </si>
   <si>
     <t>T3</t>

</xml_diff>